<commit_message>
Updated data and evaluation
</commit_message>
<xml_diff>
--- a/data/interview-data.xlsx
+++ b/data/interview-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juf\Workspace\BTH\Data Processing\rqi-pat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13863FD4-4768-459C-B9B4-66AAE1CC504F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00305A2-932F-4AEC-8A20-26E7389DFC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14805" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="208">
   <si>
     <t>ID</t>
   </si>
@@ -1210,9 +1210,9 @@
   </sheetPr>
   <dimension ref="A1:W109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA12" sqref="AA12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T63" sqref="T63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3843,7 +3843,9 @@
       <c r="S62" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="T62" s="8"/>
+      <c r="T62" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="U62" s="8"/>
       <c r="V62" s="8"/>
       <c r="W62" s="11"/>
@@ -5841,7 +5843,7 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
@@ -8479,7 +8481,7 @@
       </c>
       <c r="C3" s="6">
         <f>COUNTIF(Data!T:T, A3) + COUNTIF(Data!W:W, A3)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>